<commit_message>
add xlwings pro brief
</commit_message>
<xml_diff>
--- a/notebook/rdp_report.xlsx
+++ b/notebook/rdp_report.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6028883D-FA4F-4D4C-8F2B-622B1174CB55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6633269-2E75-4E6A-AF86-6C43BB431C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22440" yWindow="804" windowWidth="21900" windowHeight="11220" xr2:uid="{5D7D31BF-94F4-48D7-B042-D6D4DAC167C0}"/>
+    <workbookView xWindow="-23148" yWindow="-420" windowWidth="23256" windowHeight="12720" xr2:uid="{BB0AA220-49DD-4313-AD3A-29FC46E9720D}"/>
   </bookViews>
   <sheets>
-    <sheet name="VOD.L Historical Data" sheetId="1" r:id="rId1"/>
+    <sheet name="VOD.L ESG Data" sheetId="4" r:id="rId1"/>
+    <sheet name="VOD.L Historical Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>BID</t>
   </si>
@@ -60,6 +61,87 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>VOD.L Environmental, Social and Governance Scores for last 5 years</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Period End Date</t>
+  </si>
+  <si>
+    <t>ESG Combined Score</t>
+  </si>
+  <si>
+    <t>ESG Score</t>
+  </si>
+  <si>
+    <t>ESG Controversies Score</t>
+  </si>
+  <si>
+    <t>Environment Pillar Score</t>
+  </si>
+  <si>
+    <t>Social Pillar Score</t>
+  </si>
+  <si>
+    <t>Governance Pillar Score</t>
+  </si>
+  <si>
+    <t>Resource Use Score</t>
+  </si>
+  <si>
+    <t>Emissions Score</t>
+  </si>
+  <si>
+    <t>Innovation Score</t>
+  </si>
+  <si>
+    <t>Workforce Score</t>
+  </si>
+  <si>
+    <t>Human Rights Score</t>
+  </si>
+  <si>
+    <t>Community Score</t>
+  </si>
+  <si>
+    <t>Product Responsibility Score</t>
+  </si>
+  <si>
+    <t>Management Score</t>
+  </si>
+  <si>
+    <t>Shareholders Score</t>
+  </si>
+  <si>
+    <t>CSR Strategy Score</t>
+  </si>
+  <si>
+    <t>ESG Reporting Scope</t>
+  </si>
+  <si>
+    <t>ESG Report Auditor Name</t>
+  </si>
+  <si>
+    <t>ESG Period Last Update Date</t>
+  </si>
+  <si>
+    <t>VOD.L</t>
+  </si>
+  <si>
+    <t>Grant Thornton UK LLP</t>
+  </si>
+  <si>
+    <t>2020-09-18T00:00:00</t>
+  </si>
+  <si>
+    <t>KPMG LLP</t>
+  </si>
+  <si>
+    <t>Ernst &amp; Young LLP</t>
   </si>
 </sst>
 </file>
@@ -152,22 +234,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>211413</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>523825</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>151714</xdr:rowOff>
+      <xdr:rowOff>153619</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D54E8FF-33A7-4755-8821-E5C4BF7750EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ADD6587-C7D4-4795-9E11-5DAB7EC50978}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -189,8 +271,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1743075" y="6524625"/>
-          <a:ext cx="10488888" cy="5485714"/>
+          <a:off x="609601" y="6524625"/>
+          <a:ext cx="10566984" cy="5485714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -498,25 +580,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E103EF98-57C6-42B4-8909-E2CED6D4EF70}">
-  <dimension ref="A1:H32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDACC5D7-F780-45B7-B958-6AEF67C93B57}">
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="19" max="19" width="13.5703125" customWidth="1"/>
+    <col min="20" max="20" width="21.28515625" customWidth="1"/>
+    <col min="21" max="21" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -525,6 +605,504 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+    </row>
+    <row r="2" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43921</v>
+      </c>
+      <c r="C3">
+        <v>44.902141583097396</v>
+      </c>
+      <c r="D3">
+        <v>81.909546324089604</v>
+      </c>
+      <c r="E3">
+        <v>7.8947368421052602</v>
+      </c>
+      <c r="F3">
+        <v>71.026194977045606</v>
+      </c>
+      <c r="G3">
+        <v>81.6403995033954</v>
+      </c>
+      <c r="H3">
+        <v>90.793237924993505</v>
+      </c>
+      <c r="I3">
+        <v>81.521739130434696</v>
+      </c>
+      <c r="J3">
+        <v>68.796992481203006</v>
+      </c>
+      <c r="K3">
+        <v>61.578947368421098</v>
+      </c>
+      <c r="L3">
+        <v>68.934911242603505</v>
+      </c>
+      <c r="M3">
+        <v>91.869918699186897</v>
+      </c>
+      <c r="N3">
+        <v>63.609467455621299</v>
+      </c>
+      <c r="O3">
+        <v>93.081761006289298</v>
+      </c>
+      <c r="P3">
+        <v>98.769574944071493</v>
+      </c>
+      <c r="Q3">
+        <v>65.324384787471999</v>
+      </c>
+      <c r="R3">
+        <v>89.1148325358851</v>
+      </c>
+      <c r="S3">
+        <v>100</v>
+      </c>
+      <c r="T3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43555</v>
+      </c>
+      <c r="C4">
+        <v>46.876659018062398</v>
+      </c>
+      <c r="D4">
+        <v>79.467603750410603</v>
+      </c>
+      <c r="E4">
+        <v>14.285714285714199</v>
+      </c>
+      <c r="F4">
+        <v>74.162322155360499</v>
+      </c>
+      <c r="G4">
+        <v>84.343226376576098</v>
+      </c>
+      <c r="H4">
+        <v>73.756654261917404</v>
+      </c>
+      <c r="I4">
+        <v>88.686131386861305</v>
+      </c>
+      <c r="J4">
+        <v>70.075757575757507</v>
+      </c>
+      <c r="K4">
+        <v>62.234042553191401</v>
+      </c>
+      <c r="L4">
+        <v>78.529411764705799</v>
+      </c>
+      <c r="M4">
+        <v>91.869918699186897</v>
+      </c>
+      <c r="N4">
+        <v>65</v>
+      </c>
+      <c r="O4">
+        <v>93.081761006289298</v>
+      </c>
+      <c r="P4">
+        <v>80.5555555555555</v>
+      </c>
+      <c r="Q4">
+        <v>41.3333333333333</v>
+      </c>
+      <c r="R4">
+        <v>88.397129186602797</v>
+      </c>
+      <c r="S4">
+        <v>100</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43190</v>
+      </c>
+      <c r="C5">
+        <v>66.434472610463402</v>
+      </c>
+      <c r="D5">
+        <v>80.429920830683102</v>
+      </c>
+      <c r="E5">
+        <v>52.439024390243901</v>
+      </c>
+      <c r="F5">
+        <v>71.208572538382498</v>
+      </c>
+      <c r="G5">
+        <v>85.562144196159394</v>
+      </c>
+      <c r="H5">
+        <v>77.206662105130206</v>
+      </c>
+      <c r="I5">
+        <v>89.370078740157396</v>
+      </c>
+      <c r="J5">
+        <v>60.546875</v>
+      </c>
+      <c r="K5">
+        <v>62.6373626373626</v>
+      </c>
+      <c r="L5">
+        <v>80.538922155688596</v>
+      </c>
+      <c r="M5">
+        <v>92.4778761061946</v>
+      </c>
+      <c r="N5">
+        <v>65.568862275449106</v>
+      </c>
+      <c r="O5">
+        <v>94.516129032258107</v>
+      </c>
+      <c r="P5">
+        <v>84.920634920634896</v>
+      </c>
+      <c r="Q5">
+        <v>43.197278911564602</v>
+      </c>
+      <c r="R5">
+        <v>89.650872817955104</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+      <c r="T5" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1">
+        <v>42825</v>
+      </c>
+      <c r="C6">
+        <v>45.432762203137699</v>
+      </c>
+      <c r="D6">
+        <v>83.921079961831097</v>
+      </c>
+      <c r="E6">
+        <v>6.9444444444444402</v>
+      </c>
+      <c r="F6">
+        <v>70.969890603143995</v>
+      </c>
+      <c r="G6">
+        <v>85.947714012021706</v>
+      </c>
+      <c r="H6">
+        <v>89.785797958386695</v>
+      </c>
+      <c r="I6">
+        <v>88.842975206611499</v>
+      </c>
+      <c r="J6">
+        <v>59.426229508196698</v>
+      </c>
+      <c r="K6">
+        <v>63.736263736263702</v>
+      </c>
+      <c r="L6">
+        <v>92.236024844720504</v>
+      </c>
+      <c r="M6">
+        <v>92.5</v>
+      </c>
+      <c r="N6">
+        <v>48.7577639751552</v>
+      </c>
+      <c r="O6">
+        <v>95.033112582781399</v>
+      </c>
+      <c r="P6">
+        <v>89.720812182741099</v>
+      </c>
+      <c r="Q6">
+        <v>92.258883248730896</v>
+      </c>
+      <c r="R6">
+        <v>86.401098901098905</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+      <c r="T6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42460</v>
+      </c>
+      <c r="C7">
+        <v>80.9121465611709</v>
+      </c>
+      <c r="D7">
+        <v>80.9121465611709</v>
+      </c>
+      <c r="E7">
+        <v>87.878787878787804</v>
+      </c>
+      <c r="F7">
+        <v>69.296119203825199</v>
+      </c>
+      <c r="G7">
+        <v>85.228714467924803</v>
+      </c>
+      <c r="H7">
+        <v>81.160650788812902</v>
+      </c>
+      <c r="I7">
+        <v>88.260869565217305</v>
+      </c>
+      <c r="J7">
+        <v>54.347826086956502</v>
+      </c>
+      <c r="K7">
+        <v>64.705882352941103</v>
+      </c>
+      <c r="L7">
+        <v>90.522875816993405</v>
+      </c>
+      <c r="M7">
+        <v>94.827586206896498</v>
+      </c>
+      <c r="N7">
+        <v>45.424836601307099</v>
+      </c>
+      <c r="O7">
+        <v>93.928571428571402</v>
+      </c>
+      <c r="P7">
+        <v>76.295336787564693</v>
+      </c>
+      <c r="Q7">
+        <v>93.782383419689097</v>
+      </c>
+      <c r="R7">
+        <v>86.554621848739501</v>
+      </c>
+      <c r="S7">
+        <v>100</v>
+      </c>
+      <c r="T7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42094</v>
+      </c>
+      <c r="C8">
+        <v>45.114530190520099</v>
+      </c>
+      <c r="D8">
+        <v>88.145727047706899</v>
+      </c>
+      <c r="E8">
+        <v>2.0833333333333299</v>
+      </c>
+      <c r="F8">
+        <v>72.615361131217497</v>
+      </c>
+      <c r="G8">
+        <v>92.471247053196606</v>
+      </c>
+      <c r="H8">
+        <v>91.377270239339197</v>
+      </c>
+      <c r="I8">
+        <v>88.938053097345104</v>
+      </c>
+      <c r="J8">
+        <v>60.267857142857103</v>
+      </c>
+      <c r="K8">
+        <v>68.072289156626496</v>
+      </c>
+      <c r="L8">
+        <v>88.848920863309303</v>
+      </c>
+      <c r="M8">
+        <v>95.294117647058798</v>
+      </c>
+      <c r="N8">
+        <v>88.848920863309303</v>
+      </c>
+      <c r="O8">
+        <v>95</v>
+      </c>
+      <c r="P8">
+        <v>94.415584415584405</v>
+      </c>
+      <c r="Q8">
+        <v>84.025974025973994</v>
+      </c>
+      <c r="R8">
+        <v>87.212643678160902</v>
+      </c>
+      <c r="S8">
+        <v>100</v>
+      </c>
+      <c r="T8" t="s">
+        <v>35</v>
+      </c>
+      <c r="U8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C61BECC-17D1-4401-83F1-069A54DE7B08}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -554,782 +1132,782 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43985</v>
+        <v>43986</v>
       </c>
       <c r="B3">
-        <v>136.54</v>
+        <v>137.12</v>
       </c>
       <c r="C3">
-        <v>136.58000000000001</v>
+        <v>137.16</v>
       </c>
       <c r="D3">
-        <v>135.1</v>
+        <v>135.80000000000001</v>
       </c>
       <c r="E3">
-        <v>136.66</v>
+        <v>137.44</v>
       </c>
       <c r="F3">
-        <v>133.38</v>
+        <v>134.86000000000001</v>
       </c>
       <c r="G3">
-        <v>134.04</v>
+        <v>137.16</v>
       </c>
       <c r="H3">
-        <v>17076</v>
+        <v>10010</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="B4">
-        <v>137.12</v>
+        <v>138.94</v>
       </c>
       <c r="C4">
-        <v>137.16</v>
+        <v>138.96</v>
       </c>
       <c r="D4">
-        <v>135.80000000000001</v>
+        <v>137.5</v>
       </c>
       <c r="E4">
-        <v>137.44</v>
+        <v>139.08000000000001</v>
       </c>
       <c r="F4">
-        <v>134.86000000000001</v>
+        <v>136.08000000000001</v>
       </c>
       <c r="G4">
-        <v>137.16</v>
+        <v>138.96</v>
       </c>
       <c r="H4">
-        <v>10010</v>
+        <v>11592</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43987</v>
+        <v>43990</v>
       </c>
       <c r="B5">
-        <v>138.94</v>
+        <v>141.12</v>
       </c>
       <c r="C5">
-        <v>138.96</v>
+        <v>141.13999999999999</v>
       </c>
       <c r="D5">
-        <v>137.5</v>
+        <v>137.34</v>
       </c>
       <c r="E5">
-        <v>139.08000000000001</v>
+        <v>142.44</v>
       </c>
       <c r="F5">
-        <v>136.08000000000001</v>
+        <v>137.04</v>
       </c>
       <c r="G5">
-        <v>138.96</v>
+        <v>141.58000000000001</v>
       </c>
       <c r="H5">
-        <v>11592</v>
+        <v>15718</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="B6">
-        <v>141.12</v>
+        <v>138.94</v>
       </c>
       <c r="C6">
-        <v>141.13999999999999</v>
+        <v>139</v>
       </c>
       <c r="D6">
-        <v>137.34</v>
+        <v>140.52000000000001</v>
       </c>
       <c r="E6">
-        <v>142.44</v>
+        <v>141.66</v>
       </c>
       <c r="F6">
-        <v>137.04</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="G6">
-        <v>141.58000000000001</v>
+        <v>139.67169999999999</v>
       </c>
       <c r="H6">
-        <v>15718</v>
+        <v>16127</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="B7">
-        <v>138.94</v>
+        <v>136.26</v>
       </c>
       <c r="C7">
-        <v>139</v>
+        <v>136.28</v>
       </c>
       <c r="D7">
-        <v>140.52000000000001</v>
+        <v>138.02000000000001</v>
       </c>
       <c r="E7">
-        <v>141.66</v>
+        <v>138.63999999999999</v>
       </c>
       <c r="F7">
-        <v>138.30000000000001</v>
+        <v>135.28</v>
       </c>
       <c r="G7">
-        <v>139.67169999999999</v>
+        <v>136.74809999999999</v>
       </c>
       <c r="H7">
-        <v>16127</v>
+        <v>18794</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="B8">
-        <v>136.26</v>
+        <v>125.84</v>
       </c>
       <c r="C8">
-        <v>136.28</v>
+        <v>125.94</v>
       </c>
       <c r="D8">
-        <v>138.02000000000001</v>
+        <v>131.47999999999999</v>
       </c>
       <c r="E8">
-        <v>138.63999999999999</v>
+        <v>132.38</v>
       </c>
       <c r="F8">
-        <v>135.28</v>
+        <v>125.94</v>
       </c>
       <c r="G8">
-        <v>136.74809999999999</v>
+        <v>126.66379999999999</v>
       </c>
       <c r="H8">
-        <v>18794</v>
+        <v>19040</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="B9">
-        <v>125.84</v>
+        <v>126.08</v>
       </c>
       <c r="C9">
-        <v>125.94</v>
+        <v>126.1</v>
       </c>
       <c r="D9">
-        <v>131.47999999999999</v>
+        <v>124.66</v>
       </c>
       <c r="E9">
-        <v>132.38</v>
+        <v>127.9</v>
       </c>
       <c r="F9">
-        <v>125.94</v>
+        <v>122.24</v>
       </c>
       <c r="G9">
-        <v>126.66379999999999</v>
+        <v>126.1</v>
       </c>
       <c r="H9">
-        <v>19040</v>
+        <v>16595</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43994</v>
+        <v>43997</v>
       </c>
       <c r="B10">
-        <v>126.08</v>
+        <v>124.44</v>
       </c>
       <c r="C10">
-        <v>126.1</v>
+        <v>124.46</v>
       </c>
       <c r="D10">
-        <v>124.66</v>
+        <v>123.76</v>
       </c>
       <c r="E10">
-        <v>127.9</v>
+        <v>125.06</v>
       </c>
       <c r="F10">
-        <v>122.24</v>
+        <v>122.7</v>
       </c>
       <c r="G10">
-        <v>126.1</v>
+        <v>124.46</v>
       </c>
       <c r="H10">
-        <v>16595</v>
+        <v>13748</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="B11">
-        <v>124.44</v>
+        <v>129.1</v>
       </c>
       <c r="C11">
-        <v>124.46</v>
+        <v>129.12</v>
       </c>
       <c r="D11">
-        <v>123.76</v>
+        <v>126.94</v>
       </c>
       <c r="E11">
-        <v>125.06</v>
+        <v>130.56</v>
       </c>
       <c r="F11">
-        <v>122.7</v>
+        <v>126.2</v>
       </c>
       <c r="G11">
-        <v>124.46</v>
+        <v>128.98285999999999</v>
       </c>
       <c r="H11">
-        <v>13748</v>
+        <v>14998</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="B12">
+        <v>129.08000000000001</v>
+      </c>
+      <c r="C12">
         <v>129.1</v>
       </c>
-      <c r="C12">
-        <v>129.12</v>
-      </c>
       <c r="D12">
-        <v>126.94</v>
+        <v>129.5</v>
       </c>
       <c r="E12">
-        <v>130.56</v>
+        <v>131.06</v>
       </c>
       <c r="F12">
-        <v>126.2</v>
+        <v>128.54</v>
       </c>
       <c r="G12">
-        <v>128.98285999999999</v>
+        <v>129.1</v>
       </c>
       <c r="H12">
-        <v>14998</v>
+        <v>13539</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="B13">
-        <v>129.08000000000001</v>
+        <v>127</v>
       </c>
       <c r="C13">
-        <v>129.1</v>
+        <v>127.02</v>
       </c>
       <c r="D13">
-        <v>129.5</v>
+        <v>128.54</v>
       </c>
       <c r="E13">
-        <v>131.06</v>
+        <v>129.28</v>
       </c>
       <c r="F13">
-        <v>128.54</v>
+        <v>126.56</v>
       </c>
       <c r="G13">
-        <v>129.1</v>
+        <v>127.26</v>
       </c>
       <c r="H13">
-        <v>13539</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="B14">
-        <v>127</v>
+        <v>127.76</v>
       </c>
       <c r="C14">
-        <v>127.02</v>
+        <v>127.78</v>
       </c>
       <c r="D14">
-        <v>128.54</v>
+        <v>127.66</v>
       </c>
       <c r="E14">
-        <v>129.28</v>
+        <v>130.22</v>
       </c>
       <c r="F14">
-        <v>126.56</v>
+        <v>127.14</v>
       </c>
       <c r="G14">
-        <v>127.26</v>
+        <v>128.43521000000001</v>
       </c>
       <c r="H14">
-        <v>8733</v>
+        <v>9493</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44001</v>
+        <v>44004</v>
       </c>
       <c r="B15">
-        <v>127.76</v>
+        <v>126.78</v>
       </c>
       <c r="C15">
-        <v>127.78</v>
+        <v>126.84</v>
       </c>
       <c r="D15">
-        <v>127.66</v>
+        <v>126.86</v>
       </c>
       <c r="E15">
-        <v>130.22</v>
+        <v>128.32</v>
       </c>
       <c r="F15">
-        <v>127.14</v>
+        <v>125.86</v>
       </c>
       <c r="G15">
-        <v>128.43521000000001</v>
+        <v>126.78</v>
       </c>
       <c r="H15">
-        <v>9493</v>
+        <v>7383</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="B16">
-        <v>126.78</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="C16">
-        <v>126.84</v>
+        <v>129.16</v>
       </c>
       <c r="D16">
-        <v>126.86</v>
+        <v>127.58</v>
       </c>
       <c r="E16">
-        <v>128.32</v>
+        <v>130.72</v>
       </c>
       <c r="F16">
-        <v>125.86</v>
+        <v>127.22</v>
       </c>
       <c r="G16">
-        <v>126.78</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="H16">
-        <v>7383</v>
+        <v>11552</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="B17">
-        <v>129.13999999999999</v>
+        <v>125.02</v>
       </c>
       <c r="C17">
-        <v>129.16</v>
+        <v>125.04</v>
       </c>
       <c r="D17">
-        <v>127.58</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="E17">
-        <v>130.72</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="F17">
-        <v>127.22</v>
+        <v>124.94</v>
       </c>
       <c r="G17">
-        <v>129.13999999999999</v>
+        <v>125.04</v>
       </c>
       <c r="H17">
-        <v>11552</v>
+        <v>10019</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="B18">
-        <v>125.02</v>
+        <v>127.02</v>
       </c>
       <c r="C18">
-        <v>125.04</v>
+        <v>127.06</v>
       </c>
       <c r="D18">
-        <v>128.47999999999999</v>
+        <v>125.08</v>
       </c>
       <c r="E18">
-        <v>128.47999999999999</v>
+        <v>127.4</v>
       </c>
       <c r="F18">
-        <v>124.94</v>
+        <v>123.98</v>
       </c>
       <c r="G18">
-        <v>125.04</v>
+        <v>127.06</v>
       </c>
       <c r="H18">
-        <v>10019</v>
+        <v>10782</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="B19">
-        <v>127.02</v>
+        <v>125.24</v>
       </c>
       <c r="C19">
-        <v>127.06</v>
+        <v>125.28</v>
       </c>
       <c r="D19">
+        <v>128.04</v>
+      </c>
+      <c r="E19">
+        <v>129.13999999999999</v>
+      </c>
+      <c r="F19">
         <v>125.08</v>
       </c>
-      <c r="E19">
-        <v>127.4</v>
-      </c>
-      <c r="F19">
-        <v>123.98</v>
-      </c>
       <c r="G19">
-        <v>127.06</v>
+        <v>125.24</v>
       </c>
       <c r="H19">
-        <v>10782</v>
+        <v>14526</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="B20">
-        <v>125.24</v>
+        <v>127.76</v>
       </c>
       <c r="C20">
-        <v>125.28</v>
+        <v>127.8</v>
       </c>
       <c r="D20">
-        <v>128.04</v>
+        <v>125.02</v>
       </c>
       <c r="E20">
-        <v>129.13999999999999</v>
+        <v>127.98</v>
       </c>
       <c r="F20">
-        <v>125.08</v>
+        <v>123.76</v>
       </c>
       <c r="G20">
-        <v>125.24</v>
+        <v>127.24357999999999</v>
       </c>
       <c r="H20">
-        <v>14526</v>
+        <v>8682</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="B21">
-        <v>127.76</v>
+        <v>128.86000000000001</v>
       </c>
       <c r="C21">
-        <v>127.8</v>
+        <v>128.88</v>
       </c>
       <c r="D21">
-        <v>125.02</v>
+        <v>127.78</v>
       </c>
       <c r="E21">
-        <v>127.98</v>
+        <v>129.72</v>
       </c>
       <c r="F21">
-        <v>123.76</v>
+        <v>126.56</v>
       </c>
       <c r="G21">
-        <v>127.24357999999999</v>
+        <v>129</v>
       </c>
       <c r="H21">
-        <v>8682</v>
+        <v>13573</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="B22">
-        <v>128.86000000000001</v>
+        <v>127.8</v>
       </c>
       <c r="C22">
-        <v>128.88</v>
+        <v>127.84</v>
       </c>
       <c r="D22">
-        <v>127.78</v>
+        <v>128.38</v>
       </c>
       <c r="E22">
-        <v>129.72</v>
+        <v>129.44</v>
       </c>
       <c r="F22">
-        <v>126.56</v>
+        <v>125.84</v>
       </c>
       <c r="G22">
-        <v>129</v>
+        <v>127.82769999999999</v>
       </c>
       <c r="H22">
-        <v>13573</v>
+        <v>9737</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="B23">
-        <v>127.8</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="C23">
-        <v>127.84</v>
+        <v>129.5</v>
       </c>
       <c r="D23">
-        <v>128.38</v>
+        <v>128.97999999999999</v>
       </c>
       <c r="E23">
-        <v>129.44</v>
+        <v>131.4</v>
       </c>
       <c r="F23">
-        <v>125.84</v>
+        <v>128.24</v>
       </c>
       <c r="G23">
-        <v>127.82769999999999</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="H23">
-        <v>9737</v>
+        <v>8546</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="B24">
-        <v>129.47999999999999</v>
+        <v>129.58000000000001</v>
       </c>
       <c r="C24">
-        <v>129.5</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="D24">
-        <v>128.97999999999999</v>
+        <v>129.74</v>
       </c>
       <c r="E24">
-        <v>131.4</v>
+        <v>130.16</v>
       </c>
       <c r="F24">
-        <v>128.24</v>
+        <v>129.02000000000001</v>
       </c>
       <c r="G24">
-        <v>129.47999999999999</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H24">
-        <v>8546</v>
+        <v>5971</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44015</v>
+        <v>44018</v>
       </c>
       <c r="B25">
-        <v>129.58000000000001</v>
+        <v>130.24</v>
       </c>
       <c r="C25">
-        <v>129.63999999999999</v>
+        <v>130.36000000000001</v>
       </c>
       <c r="D25">
-        <v>129.74</v>
+        <v>131.52000000000001</v>
       </c>
       <c r="E25">
-        <v>130.16</v>
+        <v>131.96</v>
       </c>
       <c r="F25">
-        <v>129.02000000000001</v>
+        <v>129.88</v>
       </c>
       <c r="G25">
-        <v>129.63999999999999</v>
+        <v>130.32</v>
       </c>
       <c r="H25">
-        <v>5971</v>
+        <v>9212</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="B26">
-        <v>130.24</v>
+        <v>127.02</v>
       </c>
       <c r="C26">
-        <v>130.36000000000001</v>
+        <v>127.04</v>
       </c>
       <c r="D26">
-        <v>131.52000000000001</v>
+        <v>130.08000000000001</v>
       </c>
       <c r="E26">
-        <v>131.96</v>
+        <v>130.32</v>
       </c>
       <c r="F26">
-        <v>129.88</v>
+        <v>126.98</v>
       </c>
       <c r="G26">
-        <v>130.32</v>
+        <v>127.02</v>
       </c>
       <c r="H26">
-        <v>9212</v>
+        <v>8403</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="B27">
-        <v>127.02</v>
+        <v>125.28</v>
       </c>
       <c r="C27">
-        <v>127.04</v>
+        <v>125.3</v>
       </c>
       <c r="D27">
-        <v>130.08000000000001</v>
+        <v>126.26</v>
       </c>
       <c r="E27">
-        <v>130.32</v>
+        <v>128.08000000000001</v>
       </c>
       <c r="F27">
-        <v>126.98</v>
+        <v>125.1</v>
       </c>
       <c r="G27">
-        <v>127.02</v>
+        <v>125.6</v>
       </c>
       <c r="H27">
-        <v>8403</v>
+        <v>8337</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="B28">
-        <v>125.28</v>
+        <v>122.64</v>
       </c>
       <c r="C28">
-        <v>125.3</v>
+        <v>122.66</v>
       </c>
       <c r="D28">
-        <v>126.26</v>
+        <v>124.22</v>
       </c>
       <c r="E28">
-        <v>128.08000000000001</v>
+        <v>125.26</v>
       </c>
       <c r="F28">
-        <v>125.1</v>
+        <v>122.32</v>
       </c>
       <c r="G28">
-        <v>125.6</v>
+        <v>124.29640000000001</v>
       </c>
       <c r="H28">
-        <v>8337</v>
+        <v>7729</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="B29">
-        <v>122.64</v>
+        <v>123.4</v>
       </c>
       <c r="C29">
-        <v>122.66</v>
+        <v>123.42</v>
       </c>
       <c r="D29">
-        <v>124.22</v>
+        <v>122.08</v>
       </c>
       <c r="E29">
-        <v>125.26</v>
+        <v>123.64</v>
       </c>
       <c r="F29">
-        <v>122.32</v>
+        <v>122</v>
       </c>
       <c r="G29">
-        <v>124.29640000000001</v>
+        <v>123.42</v>
       </c>
       <c r="H29">
-        <v>7729</v>
+        <v>7637</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44022</v>
+        <v>44025</v>
       </c>
       <c r="B30">
-        <v>123.4</v>
+        <v>124.68</v>
       </c>
       <c r="C30">
-        <v>123.42</v>
+        <v>124.72</v>
       </c>
       <c r="D30">
-        <v>122.08</v>
+        <v>125.3</v>
       </c>
       <c r="E30">
-        <v>123.64</v>
+        <v>125.92</v>
       </c>
       <c r="F30">
-        <v>122</v>
+        <v>124.04</v>
       </c>
       <c r="G30">
-        <v>123.42</v>
+        <v>124.72</v>
       </c>
       <c r="H30">
-        <v>7637</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>44025</v>
+        <v>44026</v>
       </c>
       <c r="B31">
-        <v>124.68</v>
+        <v>126.9</v>
       </c>
       <c r="C31">
-        <v>124.72</v>
+        <v>126.92</v>
       </c>
       <c r="D31">
-        <v>125.3</v>
+        <v>124.14</v>
       </c>
       <c r="E31">
-        <v>125.92</v>
+        <v>128.16</v>
       </c>
       <c r="F31">
-        <v>124.04</v>
+        <v>122.94</v>
       </c>
       <c r="G31">
-        <v>124.72</v>
+        <v>126.79657</v>
       </c>
       <c r="H31">
-        <v>7585</v>
+        <v>12439</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B32">
-        <v>126.9</v>
+        <v>127.5</v>
       </c>
       <c r="C32">
-        <v>126.92</v>
+        <v>127.54</v>
       </c>
       <c r="D32">
-        <v>124.14</v>
+        <v>127.5</v>
       </c>
       <c r="E32">
-        <v>128.16</v>
+        <v>127.86</v>
       </c>
       <c r="F32">
-        <v>122.94</v>
+        <v>124.72</v>
       </c>
       <c r="G32">
-        <v>126.79657</v>
+        <v>126.855</v>
       </c>
       <c r="H32">
-        <v>12439</v>
+        <v>12158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change logs: 1. Fix and note issues that commented by xlwings team 2. Add readme and notebook detail
</commit_message>
<xml_diff>
--- a/notebook/rdp_report.xlsx
+++ b/notebook/rdp_report.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_project\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6633269-2E75-4E6A-AF86-6C43BB431C1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C40FFF14-9929-4BF5-A632-8B212146F8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-420" windowWidth="23256" windowHeight="12720" xr2:uid="{BB0AA220-49DD-4313-AD3A-29FC46E9720D}"/>
+    <workbookView xWindow="-23148" yWindow="-420" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{4CBC5942-915D-4B88-BA02-8321DABF97AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="VOD.L ESG Data" sheetId="4" r:id="rId1"/>
+    <sheet name="VOD.L ESG Data" sheetId="2" r:id="rId1"/>
     <sheet name="VOD.L Historical Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -234,22 +234,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>523825</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>153619</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>2842</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>46277</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4ADD6587-C7D4-4795-9E11-5DAB7EC50978}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D45D571-A8A4-410C-A124-AC3A451FE882}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -258,7 +258,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -271,8 +271,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609601" y="6524625"/>
-          <a:ext cx="10566984" cy="5485714"/>
+          <a:off x="609600" y="6524625"/>
+          <a:ext cx="7318042" cy="3854372"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -580,18 +580,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDACC5D7-F780-45B7-B958-6AEF67C93B57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6E7842-6A6B-41C9-B8FF-FFD78F20E975}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" customWidth="1"/>
-    <col min="20" max="20" width="21.28515625" customWidth="1"/>
-    <col min="21" max="21" width="27.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -692,52 +698,52 @@
         <v>43921</v>
       </c>
       <c r="C3">
-        <v>44.902141583097396</v>
+        <v>44.887475701770001</v>
       </c>
       <c r="D3">
-        <v>81.909546324089604</v>
+        <v>82.016330713884798</v>
       </c>
       <c r="E3">
-        <v>7.8947368421052602</v>
+        <v>7.7586206896551699</v>
       </c>
       <c r="F3">
-        <v>71.026194977045606</v>
+        <v>70.978076413478703</v>
       </c>
       <c r="G3">
-        <v>81.6403995033954</v>
+        <v>81.669384719772694</v>
       </c>
       <c r="H3">
-        <v>90.793237924993505</v>
+        <v>90.978733378792995</v>
       </c>
       <c r="I3">
-        <v>81.521739130434696</v>
+        <v>81.654676258992794</v>
       </c>
       <c r="J3">
-        <v>68.796992481203006</v>
+        <v>68.283582089552198</v>
       </c>
       <c r="K3">
-        <v>61.578947368421098</v>
+        <v>61.855670103092699</v>
       </c>
       <c r="L3">
-        <v>68.934911242603505</v>
+        <v>69.117647058823493</v>
       </c>
       <c r="M3">
-        <v>91.869918699186897</v>
+        <v>91.935483870967701</v>
       </c>
       <c r="N3">
-        <v>63.609467455621299</v>
+        <v>63.823529411764703</v>
       </c>
       <c r="O3">
-        <v>93.081761006289298</v>
+        <v>93.167701863353997</v>
       </c>
       <c r="P3">
-        <v>98.769574944071493</v>
+        <v>98.995535714285694</v>
       </c>
       <c r="Q3">
-        <v>65.324384787471999</v>
+        <v>65.401785714285694</v>
       </c>
       <c r="R3">
-        <v>89.1148325358851</v>
+        <v>89.260143198090603</v>
       </c>
       <c r="S3">
         <v>100</v>
@@ -757,52 +763,52 @@
         <v>43555</v>
       </c>
       <c r="C4">
-        <v>46.876659018062398</v>
+        <v>46.7001752693279</v>
       </c>
       <c r="D4">
-        <v>79.467603750410603</v>
+        <v>79.365262819357497</v>
       </c>
       <c r="E4">
-        <v>14.285714285714199</v>
+        <v>14.0350877192982</v>
       </c>
       <c r="F4">
-        <v>74.162322155360499</v>
+        <v>73.798477867152798</v>
       </c>
       <c r="G4">
-        <v>84.343226376576098</v>
+        <v>84.356493970821106</v>
       </c>
       <c r="H4">
-        <v>73.756654261917404</v>
+        <v>73.622939917834799</v>
       </c>
       <c r="I4">
         <v>88.686131386861305</v>
       </c>
       <c r="J4">
-        <v>70.075757575757507</v>
+        <v>68.796992481203006</v>
       </c>
       <c r="K4">
-        <v>62.234042553191401</v>
+        <v>62.5</v>
       </c>
       <c r="L4">
-        <v>78.529411764705799</v>
+        <v>78.654970760233894</v>
       </c>
       <c r="M4">
-        <v>91.869918699186897</v>
+        <v>91.935483870967701</v>
       </c>
       <c r="N4">
-        <v>65</v>
+        <v>64.619883040935605</v>
       </c>
       <c r="O4">
-        <v>93.081761006289298</v>
+        <v>93.167701863353997</v>
       </c>
       <c r="P4">
-        <v>80.5555555555555</v>
+        <v>80.376940133037607</v>
       </c>
       <c r="Q4">
-        <v>41.3333333333333</v>
+        <v>41.241685144124098</v>
       </c>
       <c r="R4">
-        <v>88.397129186602797</v>
+        <v>88.424821002386594</v>
       </c>
       <c r="S4">
         <v>100</v>
@@ -822,22 +828,22 @@
         <v>43190</v>
       </c>
       <c r="C5">
-        <v>66.434472610463402</v>
+        <v>65.820888564213007</v>
       </c>
       <c r="D5">
-        <v>80.429920830683102</v>
+        <v>80.451300937949796</v>
       </c>
       <c r="E5">
-        <v>52.439024390243901</v>
+        <v>51.190476190476097</v>
       </c>
       <c r="F5">
-        <v>71.208572538382498</v>
+        <v>71.166766518315598</v>
       </c>
       <c r="G5">
-        <v>85.562144196159394</v>
+        <v>85.665270161040496</v>
       </c>
       <c r="H5">
-        <v>77.206662105130206</v>
+        <v>77.112539051137603</v>
       </c>
       <c r="I5">
         <v>89.370078740157396</v>
@@ -846,28 +852,28 @@
         <v>60.546875</v>
       </c>
       <c r="K5">
-        <v>62.6373626373626</v>
+        <v>62.5</v>
       </c>
       <c r="L5">
-        <v>80.538922155688596</v>
+        <v>80.654761904761898</v>
       </c>
       <c r="M5">
-        <v>92.4778761061946</v>
+        <v>92.543859649122794</v>
       </c>
       <c r="N5">
-        <v>65.568862275449106</v>
+        <v>65.773809523809504</v>
       </c>
       <c r="O5">
-        <v>94.516129032258107</v>
+        <v>94.585987261146499</v>
       </c>
       <c r="P5">
-        <v>84.920634920634896</v>
+        <v>84.851936218678802</v>
       </c>
       <c r="Q5">
-        <v>43.197278911564602</v>
+        <v>42.938496583143497</v>
       </c>
       <c r="R5">
-        <v>89.650872817955104</v>
+        <v>89.676616915422798</v>
       </c>
       <c r="S5">
         <v>100</v>
@@ -887,22 +893,22 @@
         <v>42825</v>
       </c>
       <c r="C6">
-        <v>45.432762203137699</v>
+        <v>45.321783061840101</v>
       </c>
       <c r="D6">
-        <v>83.921079961831097</v>
+        <v>83.886809366923401</v>
       </c>
       <c r="E6">
-        <v>6.9444444444444402</v>
+        <v>6.7567567567567499</v>
       </c>
       <c r="F6">
-        <v>70.969890603143995</v>
+        <v>70.924449276984305</v>
       </c>
       <c r="G6">
-        <v>85.947714012021706</v>
+        <v>85.949927755797603</v>
       </c>
       <c r="H6">
-        <v>89.785797958386695</v>
+        <v>89.686920222634498</v>
       </c>
       <c r="I6">
         <v>88.842975206611499</v>
@@ -911,28 +917,28 @@
         <v>59.426229508196698</v>
       </c>
       <c r="K6">
-        <v>63.736263736263702</v>
+        <v>63.586956521739097</v>
       </c>
       <c r="L6">
-        <v>92.236024844720504</v>
+        <v>92.283950617283907</v>
       </c>
       <c r="M6">
-        <v>92.5</v>
+        <v>92.574257425742502</v>
       </c>
       <c r="N6">
-        <v>48.7577639751552</v>
+        <v>48.456790123456699</v>
       </c>
       <c r="O6">
-        <v>95.033112582781399</v>
+        <v>95.0980392156862</v>
       </c>
       <c r="P6">
-        <v>89.720812182741099</v>
+        <v>89.668367346938695</v>
       </c>
       <c r="Q6">
-        <v>92.258883248730896</v>
+        <v>91.964285714285694</v>
       </c>
       <c r="R6">
-        <v>86.401098901098905</v>
+        <v>86.363636363636303</v>
       </c>
       <c r="S6">
         <v>100</v>
@@ -952,10 +958,10 @@
         <v>42460</v>
       </c>
       <c r="C7">
-        <v>80.9121465611709</v>
+        <v>80.876741933063599</v>
       </c>
       <c r="D7">
-        <v>80.9121465611709</v>
+        <v>80.876741933063599</v>
       </c>
       <c r="E7">
         <v>87.878787878787804</v>
@@ -964,10 +970,10 @@
         <v>69.296119203825199</v>
       </c>
       <c r="G7">
-        <v>85.228714467924803</v>
+        <v>85.208902570748904</v>
       </c>
       <c r="H7">
-        <v>81.160650788812902</v>
+        <v>81.066830524344496</v>
       </c>
       <c r="I7">
         <v>88.260869565217305</v>
@@ -979,25 +985,25 @@
         <v>64.705882352941103</v>
       </c>
       <c r="L7">
-        <v>90.522875816993405</v>
+        <v>90.584415584415495</v>
       </c>
       <c r="M7">
         <v>94.827586206896498</v>
       </c>
       <c r="N7">
-        <v>45.424836601307099</v>
+        <v>45.129870129870099</v>
       </c>
       <c r="O7">
-        <v>93.928571428571402</v>
+        <v>93.971631205673702</v>
       </c>
       <c r="P7">
-        <v>76.295336787564693</v>
+        <v>76.171875</v>
       </c>
       <c r="Q7">
-        <v>93.782383419689097</v>
+        <v>93.75</v>
       </c>
       <c r="R7">
-        <v>86.554621848739501</v>
+        <v>86.516853932584198</v>
       </c>
       <c r="S7">
         <v>100</v>
@@ -1017,10 +1023,10 @@
         <v>42094</v>
       </c>
       <c r="C8">
-        <v>45.114530190520099</v>
+        <v>45.158127497665099</v>
       </c>
       <c r="D8">
-        <v>88.145727047706899</v>
+        <v>88.232921661996798</v>
       </c>
       <c r="E8">
         <v>2.0833333333333299</v>
@@ -1029,10 +1035,10 @@
         <v>72.615361131217497</v>
       </c>
       <c r="G8">
-        <v>92.471247053196606</v>
+        <v>92.5168463486132</v>
       </c>
       <c r="H8">
-        <v>91.377270239339197</v>
+        <v>91.614735780769095</v>
       </c>
       <c r="I8">
         <v>88.938053097345104</v>
@@ -1044,25 +1050,25 @@
         <v>68.072289156626496</v>
       </c>
       <c r="L8">
-        <v>88.848920863309303</v>
+        <v>88.928571428571402</v>
       </c>
       <c r="M8">
         <v>95.294117647058798</v>
       </c>
       <c r="N8">
-        <v>88.848920863309303</v>
+        <v>88.928571428571402</v>
       </c>
       <c r="O8">
-        <v>95</v>
+        <v>95.038167938931295</v>
       </c>
       <c r="P8">
-        <v>94.415584415584405</v>
+        <v>94.647519582245394</v>
       </c>
       <c r="Q8">
-        <v>84.025974025973994</v>
+        <v>84.464751958224497</v>
       </c>
       <c r="R8">
-        <v>87.212643678160902</v>
+        <v>87.175792507204605</v>
       </c>
       <c r="S8">
         <v>100</v>
@@ -1080,17 +1086,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C61BECC-17D1-4401-83F1-069A54DE7B08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A5C99A-59E0-4F4D-8273-71CD938CAF41}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -1132,787 +1133,786 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43986</v>
+        <v>43991</v>
       </c>
       <c r="B3">
-        <v>137.12</v>
+        <v>138.94</v>
       </c>
       <c r="C3">
-        <v>137.16</v>
+        <v>139</v>
       </c>
       <c r="D3">
-        <v>135.80000000000001</v>
+        <v>140.52000000000001</v>
       </c>
       <c r="E3">
-        <v>137.44</v>
+        <v>141.66</v>
       </c>
       <c r="F3">
-        <v>134.86000000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="G3">
-        <v>137.16</v>
+        <v>139.67169999999999</v>
       </c>
       <c r="H3">
-        <v>10010</v>
+        <v>16127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43987</v>
+        <v>43992</v>
       </c>
       <c r="B4">
-        <v>138.94</v>
+        <v>136.26</v>
       </c>
       <c r="C4">
-        <v>138.96</v>
+        <v>136.28</v>
       </c>
       <c r="D4">
-        <v>137.5</v>
+        <v>138.02000000000001</v>
       </c>
       <c r="E4">
-        <v>139.08000000000001</v>
+        <v>138.63999999999999</v>
       </c>
       <c r="F4">
-        <v>136.08000000000001</v>
+        <v>135.28</v>
       </c>
       <c r="G4">
-        <v>138.96</v>
+        <v>136.74809999999999</v>
       </c>
       <c r="H4">
-        <v>11592</v>
+        <v>18794</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43990</v>
+        <v>43993</v>
       </c>
       <c r="B5">
-        <v>141.12</v>
+        <v>125.84</v>
       </c>
       <c r="C5">
-        <v>141.13999999999999</v>
+        <v>125.94</v>
       </c>
       <c r="D5">
-        <v>137.34</v>
+        <v>131.47999999999999</v>
       </c>
       <c r="E5">
-        <v>142.44</v>
+        <v>132.38</v>
       </c>
       <c r="F5">
-        <v>137.04</v>
+        <v>125.94</v>
       </c>
       <c r="G5">
-        <v>141.58000000000001</v>
+        <v>126.66379999999999</v>
       </c>
       <c r="H5">
-        <v>15718</v>
+        <v>19040</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43991</v>
+        <v>43994</v>
       </c>
       <c r="B6">
-        <v>138.94</v>
+        <v>126.08</v>
       </c>
       <c r="C6">
-        <v>139</v>
+        <v>126.1</v>
       </c>
       <c r="D6">
-        <v>140.52000000000001</v>
+        <v>124.66</v>
       </c>
       <c r="E6">
-        <v>141.66</v>
+        <v>127.9</v>
       </c>
       <c r="F6">
-        <v>138.30000000000001</v>
+        <v>122.24</v>
       </c>
       <c r="G6">
-        <v>139.67169999999999</v>
+        <v>126.1</v>
       </c>
       <c r="H6">
-        <v>16127</v>
+        <v>16595</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43992</v>
+        <v>43997</v>
       </c>
       <c r="B7">
-        <v>136.26</v>
+        <v>124.44</v>
       </c>
       <c r="C7">
-        <v>136.28</v>
+        <v>124.46</v>
       </c>
       <c r="D7">
-        <v>138.02000000000001</v>
+        <v>123.76</v>
       </c>
       <c r="E7">
-        <v>138.63999999999999</v>
+        <v>125.06</v>
       </c>
       <c r="F7">
-        <v>135.28</v>
+        <v>122.7</v>
       </c>
       <c r="G7">
-        <v>136.74809999999999</v>
+        <v>124.46</v>
       </c>
       <c r="H7">
-        <v>18794</v>
+        <v>13748</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43993</v>
+        <v>43998</v>
       </c>
       <c r="B8">
-        <v>125.84</v>
+        <v>129.1</v>
       </c>
       <c r="C8">
-        <v>125.94</v>
+        <v>129.12</v>
       </c>
       <c r="D8">
-        <v>131.47999999999999</v>
+        <v>126.94</v>
       </c>
       <c r="E8">
-        <v>132.38</v>
+        <v>130.56</v>
       </c>
       <c r="F8">
-        <v>125.94</v>
+        <v>126.2</v>
       </c>
       <c r="G8">
-        <v>126.66379999999999</v>
+        <v>128.98285999999999</v>
       </c>
       <c r="H8">
-        <v>19040</v>
+        <v>14998</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43994</v>
+        <v>43999</v>
       </c>
       <c r="B9">
-        <v>126.08</v>
+        <v>129.08000000000001</v>
       </c>
       <c r="C9">
-        <v>126.1</v>
+        <v>129.1</v>
       </c>
       <c r="D9">
-        <v>124.66</v>
+        <v>129.5</v>
       </c>
       <c r="E9">
-        <v>127.9</v>
+        <v>131.06</v>
       </c>
       <c r="F9">
-        <v>122.24</v>
+        <v>128.54</v>
       </c>
       <c r="G9">
-        <v>126.1</v>
+        <v>129.1</v>
       </c>
       <c r="H9">
-        <v>16595</v>
+        <v>13539</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43997</v>
+        <v>44000</v>
       </c>
       <c r="B10">
-        <v>124.44</v>
+        <v>127</v>
       </c>
       <c r="C10">
-        <v>124.46</v>
+        <v>127.02</v>
       </c>
       <c r="D10">
-        <v>123.76</v>
+        <v>128.54</v>
       </c>
       <c r="E10">
-        <v>125.06</v>
+        <v>129.28</v>
       </c>
       <c r="F10">
-        <v>122.7</v>
+        <v>126.56</v>
       </c>
       <c r="G10">
-        <v>124.46</v>
+        <v>127.26</v>
       </c>
       <c r="H10">
-        <v>13748</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43998</v>
+        <v>44001</v>
       </c>
       <c r="B11">
-        <v>129.1</v>
+        <v>127.76</v>
       </c>
       <c r="C11">
-        <v>129.12</v>
+        <v>127.78</v>
       </c>
       <c r="D11">
-        <v>126.94</v>
+        <v>127.66</v>
       </c>
       <c r="E11">
-        <v>130.56</v>
+        <v>130.22</v>
       </c>
       <c r="F11">
-        <v>126.2</v>
+        <v>127.14</v>
       </c>
       <c r="G11">
-        <v>128.98285999999999</v>
+        <v>128.43521000000001</v>
       </c>
       <c r="H11">
-        <v>14998</v>
+        <v>9493</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43999</v>
+        <v>44004</v>
       </c>
       <c r="B12">
-        <v>129.08000000000001</v>
+        <v>126.78</v>
       </c>
       <c r="C12">
-        <v>129.1</v>
+        <v>126.84</v>
       </c>
       <c r="D12">
-        <v>129.5</v>
+        <v>126.86</v>
       </c>
       <c r="E12">
-        <v>131.06</v>
+        <v>128.32</v>
       </c>
       <c r="F12">
-        <v>128.54</v>
+        <v>125.86</v>
       </c>
       <c r="G12">
-        <v>129.1</v>
+        <v>126.78</v>
       </c>
       <c r="H12">
-        <v>13539</v>
+        <v>7383</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44000</v>
+        <v>44005</v>
       </c>
       <c r="B13">
-        <v>127</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="C13">
-        <v>127.02</v>
+        <v>129.16</v>
       </c>
       <c r="D13">
-        <v>128.54</v>
+        <v>127.58</v>
       </c>
       <c r="E13">
-        <v>129.28</v>
+        <v>130.72</v>
       </c>
       <c r="F13">
-        <v>126.56</v>
+        <v>127.22</v>
       </c>
       <c r="G13">
-        <v>127.26</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="H13">
-        <v>8733</v>
+        <v>11552</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44001</v>
+        <v>44006</v>
       </c>
       <c r="B14">
-        <v>127.76</v>
+        <v>125.02</v>
       </c>
       <c r="C14">
-        <v>127.78</v>
+        <v>125.04</v>
       </c>
       <c r="D14">
-        <v>127.66</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="E14">
-        <v>130.22</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="F14">
-        <v>127.14</v>
+        <v>124.94</v>
       </c>
       <c r="G14">
-        <v>128.43521000000001</v>
+        <v>125.04</v>
       </c>
       <c r="H14">
-        <v>9493</v>
+        <v>10019</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44004</v>
+        <v>44007</v>
       </c>
       <c r="B15">
-        <v>126.78</v>
+        <v>127.02</v>
       </c>
       <c r="C15">
-        <v>126.84</v>
+        <v>127.06</v>
       </c>
       <c r="D15">
-        <v>126.86</v>
+        <v>125.08</v>
       </c>
       <c r="E15">
-        <v>128.32</v>
+        <v>127.4</v>
       </c>
       <c r="F15">
-        <v>125.86</v>
+        <v>123.98</v>
       </c>
       <c r="G15">
-        <v>126.78</v>
+        <v>127.06</v>
       </c>
       <c r="H15">
-        <v>7383</v>
+        <v>10782</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44005</v>
+        <v>44008</v>
       </c>
       <c r="B16">
+        <v>125.24</v>
+      </c>
+      <c r="C16">
+        <v>125.28</v>
+      </c>
+      <c r="D16">
+        <v>128.04</v>
+      </c>
+      <c r="E16">
         <v>129.13999999999999</v>
       </c>
-      <c r="C16">
-        <v>129.16</v>
-      </c>
-      <c r="D16">
-        <v>127.58</v>
-      </c>
-      <c r="E16">
-        <v>130.72</v>
-      </c>
       <c r="F16">
-        <v>127.22</v>
+        <v>125.08</v>
       </c>
       <c r="G16">
-        <v>129.13999999999999</v>
+        <v>125.24</v>
       </c>
       <c r="H16">
-        <v>11552</v>
+        <v>14526</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44006</v>
+        <v>44011</v>
       </c>
       <c r="B17">
+        <v>127.76</v>
+      </c>
+      <c r="C17">
+        <v>127.8</v>
+      </c>
+      <c r="D17">
         <v>125.02</v>
       </c>
-      <c r="C17">
-        <v>125.04</v>
-      </c>
-      <c r="D17">
-        <v>128.47999999999999</v>
-      </c>
       <c r="E17">
-        <v>128.47999999999999</v>
+        <v>127.98</v>
       </c>
       <c r="F17">
-        <v>124.94</v>
+        <v>123.76</v>
       </c>
       <c r="G17">
-        <v>125.04</v>
+        <v>127.24357999999999</v>
       </c>
       <c r="H17">
-        <v>10019</v>
+        <v>8682</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44007</v>
+        <v>44012</v>
       </c>
       <c r="B18">
-        <v>127.02</v>
+        <v>128.86000000000001</v>
       </c>
       <c r="C18">
-        <v>127.06</v>
+        <v>128.88</v>
       </c>
       <c r="D18">
-        <v>125.08</v>
+        <v>127.78</v>
       </c>
       <c r="E18">
-        <v>127.4</v>
+        <v>129.72</v>
       </c>
       <c r="F18">
-        <v>123.98</v>
+        <v>126.56</v>
       </c>
       <c r="G18">
-        <v>127.06</v>
+        <v>129</v>
       </c>
       <c r="H18">
-        <v>10782</v>
+        <v>13573</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44008</v>
+        <v>44013</v>
       </c>
       <c r="B19">
-        <v>125.24</v>
+        <v>127.8</v>
       </c>
       <c r="C19">
-        <v>125.28</v>
+        <v>127.84</v>
       </c>
       <c r="D19">
-        <v>128.04</v>
+        <v>128.38</v>
       </c>
       <c r="E19">
-        <v>129.13999999999999</v>
+        <v>129.44</v>
       </c>
       <c r="F19">
-        <v>125.08</v>
+        <v>125.84</v>
       </c>
       <c r="G19">
-        <v>125.24</v>
+        <v>127.82769999999999</v>
       </c>
       <c r="H19">
-        <v>14526</v>
+        <v>9737</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44011</v>
+        <v>44014</v>
       </c>
       <c r="B20">
-        <v>127.76</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="C20">
-        <v>127.8</v>
+        <v>129.5</v>
       </c>
       <c r="D20">
-        <v>125.02</v>
+        <v>128.97999999999999</v>
       </c>
       <c r="E20">
-        <v>127.98</v>
+        <v>131.4</v>
       </c>
       <c r="F20">
-        <v>123.76</v>
+        <v>128.24</v>
       </c>
       <c r="G20">
-        <v>127.24357999999999</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="H20">
-        <v>8682</v>
+        <v>8546</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44012</v>
+        <v>44015</v>
       </c>
       <c r="B21">
-        <v>128.86000000000001</v>
+        <v>129.58000000000001</v>
       </c>
       <c r="C21">
-        <v>128.88</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="D21">
-        <v>127.78</v>
+        <v>129.74</v>
       </c>
       <c r="E21">
-        <v>129.72</v>
+        <v>130.16</v>
       </c>
       <c r="F21">
-        <v>126.56</v>
+        <v>129.02000000000001</v>
       </c>
       <c r="G21">
-        <v>129</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H21">
-        <v>13573</v>
+        <v>5971</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44013</v>
+        <v>44018</v>
       </c>
       <c r="B22">
-        <v>127.8</v>
+        <v>130.24</v>
       </c>
       <c r="C22">
-        <v>127.84</v>
+        <v>130.36000000000001</v>
       </c>
       <c r="D22">
-        <v>128.38</v>
+        <v>131.52000000000001</v>
       </c>
       <c r="E22">
-        <v>129.44</v>
+        <v>131.96</v>
       </c>
       <c r="F22">
-        <v>125.84</v>
+        <v>129.88</v>
       </c>
       <c r="G22">
-        <v>127.82769999999999</v>
+        <v>130.32</v>
       </c>
       <c r="H22">
-        <v>9737</v>
+        <v>9212</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44014</v>
+        <v>44019</v>
       </c>
       <c r="B23">
-        <v>129.47999999999999</v>
+        <v>127.02</v>
       </c>
       <c r="C23">
-        <v>129.5</v>
+        <v>127.04</v>
       </c>
       <c r="D23">
-        <v>128.97999999999999</v>
+        <v>130.08000000000001</v>
       </c>
       <c r="E23">
-        <v>131.4</v>
+        <v>130.32</v>
       </c>
       <c r="F23">
-        <v>128.24</v>
+        <v>126.98</v>
       </c>
       <c r="G23">
-        <v>129.47999999999999</v>
+        <v>127.02</v>
       </c>
       <c r="H23">
-        <v>8546</v>
+        <v>8403</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44015</v>
+        <v>44020</v>
       </c>
       <c r="B24">
-        <v>129.58000000000001</v>
+        <v>125.28</v>
       </c>
       <c r="C24">
-        <v>129.63999999999999</v>
+        <v>125.3</v>
       </c>
       <c r="D24">
-        <v>129.74</v>
+        <v>126.26</v>
       </c>
       <c r="E24">
-        <v>130.16</v>
+        <v>128.08000000000001</v>
       </c>
       <c r="F24">
-        <v>129.02000000000001</v>
+        <v>125.1</v>
       </c>
       <c r="G24">
-        <v>129.63999999999999</v>
+        <v>125.6</v>
       </c>
       <c r="H24">
-        <v>5971</v>
+        <v>8337</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44018</v>
+        <v>44021</v>
       </c>
       <c r="B25">
-        <v>130.24</v>
+        <v>122.64</v>
       </c>
       <c r="C25">
-        <v>130.36000000000001</v>
+        <v>122.66</v>
       </c>
       <c r="D25">
-        <v>131.52000000000001</v>
+        <v>124.22</v>
       </c>
       <c r="E25">
-        <v>131.96</v>
+        <v>125.26</v>
       </c>
       <c r="F25">
-        <v>129.88</v>
+        <v>122.32</v>
       </c>
       <c r="G25">
-        <v>130.32</v>
+        <v>124.29640000000001</v>
       </c>
       <c r="H25">
-        <v>9212</v>
+        <v>7729</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44019</v>
+        <v>44022</v>
       </c>
       <c r="B26">
-        <v>127.02</v>
+        <v>123.4</v>
       </c>
       <c r="C26">
-        <v>127.04</v>
+        <v>123.42</v>
       </c>
       <c r="D26">
-        <v>130.08000000000001</v>
+        <v>122.08</v>
       </c>
       <c r="E26">
-        <v>130.32</v>
+        <v>123.64</v>
       </c>
       <c r="F26">
-        <v>126.98</v>
+        <v>122</v>
       </c>
       <c r="G26">
-        <v>127.02</v>
+        <v>123.42</v>
       </c>
       <c r="H26">
-        <v>8403</v>
+        <v>7637</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44020</v>
+        <v>44025</v>
       </c>
       <c r="B27">
-        <v>125.28</v>
+        <v>124.68</v>
       </c>
       <c r="C27">
+        <v>124.72</v>
+      </c>
+      <c r="D27">
         <v>125.3</v>
       </c>
-      <c r="D27">
-        <v>126.26</v>
-      </c>
       <c r="E27">
-        <v>128.08000000000001</v>
+        <v>125.92</v>
       </c>
       <c r="F27">
-        <v>125.1</v>
+        <v>124.04</v>
       </c>
       <c r="G27">
-        <v>125.6</v>
+        <v>124.72</v>
       </c>
       <c r="H27">
-        <v>8337</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44021</v>
+        <v>44026</v>
       </c>
       <c r="B28">
-        <v>122.64</v>
+        <v>126.9</v>
       </c>
       <c r="C28">
-        <v>122.66</v>
+        <v>126.92</v>
       </c>
       <c r="D28">
-        <v>124.22</v>
+        <v>124.14</v>
       </c>
       <c r="E28">
-        <v>125.26</v>
+        <v>128.16</v>
       </c>
       <c r="F28">
-        <v>122.32</v>
+        <v>122.94</v>
       </c>
       <c r="G28">
-        <v>124.29640000000001</v>
+        <v>126.79657</v>
       </c>
       <c r="H28">
-        <v>7729</v>
+        <v>12439</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44022</v>
+        <v>44027</v>
       </c>
       <c r="B29">
-        <v>123.4</v>
+        <v>127.5</v>
       </c>
       <c r="C29">
-        <v>123.42</v>
+        <v>127.54</v>
       </c>
       <c r="D29">
-        <v>122.08</v>
+        <v>127.5</v>
       </c>
       <c r="E29">
-        <v>123.64</v>
+        <v>127.86</v>
       </c>
       <c r="F29">
-        <v>122</v>
+        <v>124.72</v>
       </c>
       <c r="G29">
-        <v>123.42</v>
+        <v>126.855</v>
       </c>
       <c r="H29">
-        <v>7637</v>
+        <v>12158</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44025</v>
+        <v>44028</v>
       </c>
       <c r="B30">
-        <v>124.68</v>
+        <v>127.46</v>
       </c>
       <c r="C30">
-        <v>124.72</v>
+        <v>127.54</v>
       </c>
       <c r="D30">
-        <v>125.3</v>
+        <v>127.02</v>
       </c>
       <c r="E30">
-        <v>125.92</v>
+        <v>128.96</v>
       </c>
       <c r="F30">
-        <v>124.04</v>
+        <v>126.84</v>
       </c>
       <c r="G30">
-        <v>124.72</v>
+        <v>127.94</v>
       </c>
       <c r="H30">
-        <v>7585</v>
+        <v>9279</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>44026</v>
+        <v>44029</v>
       </c>
       <c r="B31">
-        <v>126.9</v>
+        <v>129.78</v>
       </c>
       <c r="C31">
-        <v>126.92</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="D31">
-        <v>124.14</v>
+        <v>127.7</v>
       </c>
       <c r="E31">
-        <v>128.16</v>
+        <v>130.47999999999999</v>
       </c>
       <c r="F31">
-        <v>122.94</v>
+        <v>126.2</v>
       </c>
       <c r="G31">
-        <v>126.79657</v>
+        <v>129.048</v>
       </c>
       <c r="H31">
-        <v>12439</v>
+        <v>12281</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>44027</v>
+        <v>44032</v>
       </c>
       <c r="B32">
-        <v>127.5</v>
+        <v>129.28</v>
       </c>
       <c r="C32">
-        <v>127.54</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="D32">
-        <v>127.5</v>
+        <v>129.84</v>
       </c>
       <c r="E32">
-        <v>127.86</v>
+        <v>130.44</v>
       </c>
       <c r="F32">
-        <v>124.72</v>
+        <v>127.94</v>
       </c>
       <c r="G32">
-        <v>126.855</v>
+        <v>129.28</v>
       </c>
       <c r="H32">
-        <v>12158</v>
+        <v>9003</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make a ready production version
</commit_message>
<xml_diff>
--- a/notebook/rdp_report.xlsx
+++ b/notebook/rdp_report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive_d\Project\Code\xlwings_project\notebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U8004042\Desktop\xlwings_Oct14\notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C40FFF14-9929-4BF5-A632-8B212146F8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C7730B0-C832-49AC-9EED-766146DA49B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-420" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{4CBC5942-915D-4B88-BA02-8321DABF97AF}"/>
+    <workbookView xWindow="-22368" yWindow="684" windowWidth="22044" windowHeight="9972" xr2:uid="{09579AC7-C5EA-4925-95BF-FC6340D2DEAA}"/>
   </bookViews>
   <sheets>
     <sheet name="VOD.L ESG Data" sheetId="2" r:id="rId1"/>
@@ -234,13 +234,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1905</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>2842</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>426098</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>46277</xdr:rowOff>
     </xdr:to>
@@ -249,7 +249,7 @@
         <xdr:cNvPr id="3" name="MyPlot">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D45D571-A8A4-410C-A124-AC3A451FE882}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78F6C559-5977-43CF-859B-0B4916A5D21E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -271,8 +271,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="6524625"/>
-          <a:ext cx="7318042" cy="3854372"/>
+          <a:off x="657225" y="6524625"/>
+          <a:ext cx="7305053" cy="3854372"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -580,23 +580,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6E7842-6A6B-41C9-B8FF-FFD78F20E975}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4D2E054-1194-49D5-B319-7FCC2B106145}">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="21" max="21" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1086,12 +1077,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A5C99A-59E0-4F4D-8273-71CD938CAF41}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E9597F-6670-417D-9C60-CEDC84131309}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -1133,786 +1132,787 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="B3">
-        <v>138.94</v>
+        <v>136.26</v>
       </c>
       <c r="C3">
-        <v>139</v>
+        <v>136.28</v>
       </c>
       <c r="D3">
-        <v>140.52000000000001</v>
+        <v>138.02000000000001</v>
       </c>
       <c r="E3">
-        <v>141.66</v>
+        <v>138.63999999999999</v>
       </c>
       <c r="F3">
-        <v>138.30000000000001</v>
+        <v>135.28</v>
       </c>
       <c r="G3">
-        <v>139.67169999999999</v>
+        <v>136.74809999999999</v>
       </c>
       <c r="H3">
-        <v>16127</v>
+        <v>18794</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="B4">
-        <v>136.26</v>
+        <v>125.84</v>
       </c>
       <c r="C4">
-        <v>136.28</v>
+        <v>125.94</v>
       </c>
       <c r="D4">
-        <v>138.02000000000001</v>
+        <v>131.47999999999999</v>
       </c>
       <c r="E4">
-        <v>138.63999999999999</v>
+        <v>132.38</v>
       </c>
       <c r="F4">
-        <v>135.28</v>
+        <v>125.94</v>
       </c>
       <c r="G4">
-        <v>136.74809999999999</v>
+        <v>126.66379999999999</v>
       </c>
       <c r="H4">
-        <v>18794</v>
+        <v>19040</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="B5">
-        <v>125.84</v>
+        <v>126.08</v>
       </c>
       <c r="C5">
-        <v>125.94</v>
+        <v>126.1</v>
       </c>
       <c r="D5">
-        <v>131.47999999999999</v>
+        <v>124.66</v>
       </c>
       <c r="E5">
-        <v>132.38</v>
+        <v>127.9</v>
       </c>
       <c r="F5">
-        <v>125.94</v>
+        <v>122.24</v>
       </c>
       <c r="G5">
-        <v>126.66379999999999</v>
+        <v>126.1</v>
       </c>
       <c r="H5">
-        <v>19040</v>
+        <v>16595</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43994</v>
+        <v>43997</v>
       </c>
       <c r="B6">
-        <v>126.08</v>
+        <v>124.44</v>
       </c>
       <c r="C6">
-        <v>126.1</v>
+        <v>124.46</v>
       </c>
       <c r="D6">
-        <v>124.66</v>
+        <v>123.76</v>
       </c>
       <c r="E6">
-        <v>127.9</v>
+        <v>125.06</v>
       </c>
       <c r="F6">
-        <v>122.24</v>
+        <v>122.7</v>
       </c>
       <c r="G6">
-        <v>126.1</v>
+        <v>124.46</v>
       </c>
       <c r="H6">
-        <v>16595</v>
+        <v>13748</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="B7">
-        <v>124.44</v>
+        <v>129.1</v>
       </c>
       <c r="C7">
-        <v>124.46</v>
+        <v>129.12</v>
       </c>
       <c r="D7">
-        <v>123.76</v>
+        <v>126.94</v>
       </c>
       <c r="E7">
-        <v>125.06</v>
+        <v>130.56</v>
       </c>
       <c r="F7">
-        <v>122.7</v>
+        <v>126.2</v>
       </c>
       <c r="G7">
-        <v>124.46</v>
+        <v>128.98285999999999</v>
       </c>
       <c r="H7">
-        <v>13748</v>
+        <v>14998</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43998</v>
+        <v>43999</v>
       </c>
       <c r="B8">
+        <v>129.08000000000001</v>
+      </c>
+      <c r="C8">
         <v>129.1</v>
       </c>
-      <c r="C8">
-        <v>129.12</v>
-      </c>
       <c r="D8">
-        <v>126.94</v>
+        <v>129.5</v>
       </c>
       <c r="E8">
-        <v>130.56</v>
+        <v>131.06</v>
       </c>
       <c r="F8">
-        <v>126.2</v>
+        <v>128.54</v>
       </c>
       <c r="G8">
-        <v>128.98285999999999</v>
+        <v>129.1</v>
       </c>
       <c r="H8">
-        <v>14998</v>
+        <v>13539</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43999</v>
+        <v>44000</v>
       </c>
       <c r="B9">
-        <v>129.08000000000001</v>
+        <v>127</v>
       </c>
       <c r="C9">
-        <v>129.1</v>
+        <v>127.02</v>
       </c>
       <c r="D9">
-        <v>129.5</v>
+        <v>128.54</v>
       </c>
       <c r="E9">
-        <v>131.06</v>
+        <v>129.28</v>
       </c>
       <c r="F9">
-        <v>128.54</v>
+        <v>126.56</v>
       </c>
       <c r="G9">
-        <v>129.1</v>
+        <v>127.26</v>
       </c>
       <c r="H9">
-        <v>13539</v>
+        <v>8733</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="B10">
-        <v>127</v>
+        <v>127.76</v>
       </c>
       <c r="C10">
-        <v>127.02</v>
+        <v>127.78</v>
       </c>
       <c r="D10">
-        <v>128.54</v>
+        <v>127.66</v>
       </c>
       <c r="E10">
-        <v>129.28</v>
+        <v>130.22</v>
       </c>
       <c r="F10">
-        <v>126.56</v>
+        <v>127.14</v>
       </c>
       <c r="G10">
-        <v>127.26</v>
+        <v>128.43521000000001</v>
       </c>
       <c r="H10">
-        <v>8733</v>
+        <v>9493</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>44001</v>
+        <v>44004</v>
       </c>
       <c r="B11">
-        <v>127.76</v>
+        <v>126.78</v>
       </c>
       <c r="C11">
-        <v>127.78</v>
+        <v>126.84</v>
       </c>
       <c r="D11">
-        <v>127.66</v>
+        <v>126.86</v>
       </c>
       <c r="E11">
-        <v>130.22</v>
+        <v>128.32</v>
       </c>
       <c r="F11">
-        <v>127.14</v>
+        <v>125.86</v>
       </c>
       <c r="G11">
-        <v>128.43521000000001</v>
+        <v>126.78</v>
       </c>
       <c r="H11">
-        <v>9493</v>
+        <v>7383</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="B12">
-        <v>126.78</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="C12">
-        <v>126.84</v>
+        <v>129.16</v>
       </c>
       <c r="D12">
-        <v>126.86</v>
+        <v>127.58</v>
       </c>
       <c r="E12">
-        <v>128.32</v>
+        <v>130.72</v>
       </c>
       <c r="F12">
-        <v>125.86</v>
+        <v>127.22</v>
       </c>
       <c r="G12">
-        <v>126.78</v>
+        <v>129.13999999999999</v>
       </c>
       <c r="H12">
-        <v>7383</v>
+        <v>11552</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="B13">
-        <v>129.13999999999999</v>
+        <v>125.02</v>
       </c>
       <c r="C13">
-        <v>129.16</v>
+        <v>125.04</v>
       </c>
       <c r="D13">
-        <v>127.58</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="E13">
-        <v>130.72</v>
+        <v>128.47999999999999</v>
       </c>
       <c r="F13">
-        <v>127.22</v>
+        <v>124.94</v>
       </c>
       <c r="G13">
-        <v>129.13999999999999</v>
+        <v>125.04</v>
       </c>
       <c r="H13">
-        <v>11552</v>
+        <v>10019</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="B14">
-        <v>125.02</v>
+        <v>127.02</v>
       </c>
       <c r="C14">
-        <v>125.04</v>
+        <v>127.06</v>
       </c>
       <c r="D14">
-        <v>128.47999999999999</v>
+        <v>125.08</v>
       </c>
       <c r="E14">
-        <v>128.47999999999999</v>
+        <v>127.4</v>
       </c>
       <c r="F14">
-        <v>124.94</v>
+        <v>123.98</v>
       </c>
       <c r="G14">
-        <v>125.04</v>
+        <v>127.06</v>
       </c>
       <c r="H14">
-        <v>10019</v>
+        <v>10782</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="B15">
-        <v>127.02</v>
+        <v>125.24</v>
       </c>
       <c r="C15">
-        <v>127.06</v>
+        <v>125.28</v>
       </c>
       <c r="D15">
+        <v>128.04</v>
+      </c>
+      <c r="E15">
+        <v>129.13999999999999</v>
+      </c>
+      <c r="F15">
         <v>125.08</v>
       </c>
-      <c r="E15">
-        <v>127.4</v>
-      </c>
-      <c r="F15">
-        <v>123.98</v>
-      </c>
       <c r="G15">
-        <v>127.06</v>
+        <v>125.24</v>
       </c>
       <c r="H15">
-        <v>10782</v>
+        <v>14526</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="B16">
-        <v>125.24</v>
+        <v>127.76</v>
       </c>
       <c r="C16">
-        <v>125.28</v>
+        <v>127.8</v>
       </c>
       <c r="D16">
-        <v>128.04</v>
+        <v>125.02</v>
       </c>
       <c r="E16">
-        <v>129.13999999999999</v>
+        <v>127.98</v>
       </c>
       <c r="F16">
-        <v>125.08</v>
+        <v>123.76</v>
       </c>
       <c r="G16">
-        <v>125.24</v>
+        <v>127.24357999999999</v>
       </c>
       <c r="H16">
-        <v>14526</v>
+        <v>8682</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="B17">
-        <v>127.76</v>
+        <v>128.86000000000001</v>
       </c>
       <c r="C17">
-        <v>127.8</v>
+        <v>128.88</v>
       </c>
       <c r="D17">
-        <v>125.02</v>
+        <v>127.78</v>
       </c>
       <c r="E17">
-        <v>127.98</v>
+        <v>129.72</v>
       </c>
       <c r="F17">
-        <v>123.76</v>
+        <v>126.56</v>
       </c>
       <c r="G17">
-        <v>127.24357999999999</v>
+        <v>129</v>
       </c>
       <c r="H17">
-        <v>8682</v>
+        <v>13573</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="B18">
-        <v>128.86000000000001</v>
+        <v>127.8</v>
       </c>
       <c r="C18">
-        <v>128.88</v>
+        <v>127.84</v>
       </c>
       <c r="D18">
-        <v>127.78</v>
+        <v>128.38</v>
       </c>
       <c r="E18">
-        <v>129.72</v>
+        <v>129.44</v>
       </c>
       <c r="F18">
-        <v>126.56</v>
+        <v>125.84</v>
       </c>
       <c r="G18">
-        <v>129</v>
+        <v>127.82769999999999</v>
       </c>
       <c r="H18">
-        <v>13573</v>
+        <v>9737</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="B19">
-        <v>127.8</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="C19">
-        <v>127.84</v>
+        <v>129.5</v>
       </c>
       <c r="D19">
-        <v>128.38</v>
+        <v>128.97999999999999</v>
       </c>
       <c r="E19">
-        <v>129.44</v>
+        <v>131.4</v>
       </c>
       <c r="F19">
-        <v>125.84</v>
+        <v>128.24</v>
       </c>
       <c r="G19">
-        <v>127.82769999999999</v>
+        <v>129.47999999999999</v>
       </c>
       <c r="H19">
-        <v>9737</v>
+        <v>8546</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="B20">
-        <v>129.47999999999999</v>
+        <v>129.58000000000001</v>
       </c>
       <c r="C20">
-        <v>129.5</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="D20">
-        <v>128.97999999999999</v>
+        <v>129.74</v>
       </c>
       <c r="E20">
-        <v>131.4</v>
+        <v>130.16</v>
       </c>
       <c r="F20">
-        <v>128.24</v>
+        <v>129.02000000000001</v>
       </c>
       <c r="G20">
-        <v>129.47999999999999</v>
+        <v>129.63999999999999</v>
       </c>
       <c r="H20">
-        <v>8546</v>
+        <v>5971</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>44015</v>
+        <v>44018</v>
       </c>
       <c r="B21">
-        <v>129.58000000000001</v>
+        <v>130.24</v>
       </c>
       <c r="C21">
-        <v>129.63999999999999</v>
+        <v>130.36000000000001</v>
       </c>
       <c r="D21">
-        <v>129.74</v>
+        <v>131.52000000000001</v>
       </c>
       <c r="E21">
-        <v>130.16</v>
+        <v>131.96</v>
       </c>
       <c r="F21">
-        <v>129.02000000000001</v>
+        <v>129.88</v>
       </c>
       <c r="G21">
-        <v>129.63999999999999</v>
+        <v>130.32</v>
       </c>
       <c r="H21">
-        <v>5971</v>
+        <v>9212</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="B22">
-        <v>130.24</v>
+        <v>127.02</v>
       </c>
       <c r="C22">
-        <v>130.36000000000001</v>
+        <v>127.04</v>
       </c>
       <c r="D22">
-        <v>131.52000000000001</v>
+        <v>130.08000000000001</v>
       </c>
       <c r="E22">
-        <v>131.96</v>
+        <v>130.32</v>
       </c>
       <c r="F22">
-        <v>129.88</v>
+        <v>126.98</v>
       </c>
       <c r="G22">
-        <v>130.32</v>
+        <v>127.02</v>
       </c>
       <c r="H22">
-        <v>9212</v>
+        <v>8403</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="B23">
-        <v>127.02</v>
+        <v>125.28</v>
       </c>
       <c r="C23">
-        <v>127.04</v>
+        <v>125.3</v>
       </c>
       <c r="D23">
-        <v>130.08000000000001</v>
+        <v>126.26</v>
       </c>
       <c r="E23">
-        <v>130.32</v>
+        <v>128.08000000000001</v>
       </c>
       <c r="F23">
-        <v>126.98</v>
+        <v>125.1</v>
       </c>
       <c r="G23">
-        <v>127.02</v>
+        <v>125.6</v>
       </c>
       <c r="H23">
-        <v>8403</v>
+        <v>8337</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="B24">
-        <v>125.28</v>
+        <v>122.64</v>
       </c>
       <c r="C24">
-        <v>125.3</v>
+        <v>122.66</v>
       </c>
       <c r="D24">
-        <v>126.26</v>
+        <v>124.22</v>
       </c>
       <c r="E24">
-        <v>128.08000000000001</v>
+        <v>125.26</v>
       </c>
       <c r="F24">
-        <v>125.1</v>
+        <v>122.32</v>
       </c>
       <c r="G24">
-        <v>125.6</v>
+        <v>124.29640000000001</v>
       </c>
       <c r="H24">
-        <v>8337</v>
+        <v>7729</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="B25">
-        <v>122.64</v>
+        <v>123.4</v>
       </c>
       <c r="C25">
-        <v>122.66</v>
+        <v>123.42</v>
       </c>
       <c r="D25">
-        <v>124.22</v>
+        <v>122.08</v>
       </c>
       <c r="E25">
-        <v>125.26</v>
+        <v>123.64</v>
       </c>
       <c r="F25">
-        <v>122.32</v>
+        <v>122</v>
       </c>
       <c r="G25">
-        <v>124.29640000000001</v>
+        <v>123.42</v>
       </c>
       <c r="H25">
-        <v>7729</v>
+        <v>7637</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>44022</v>
+        <v>44025</v>
       </c>
       <c r="B26">
-        <v>123.4</v>
+        <v>124.68</v>
       </c>
       <c r="C26">
-        <v>123.42</v>
+        <v>124.72</v>
       </c>
       <c r="D26">
-        <v>122.08</v>
+        <v>125.3</v>
       </c>
       <c r="E26">
-        <v>123.64</v>
+        <v>125.92</v>
       </c>
       <c r="F26">
-        <v>122</v>
+        <v>124.04</v>
       </c>
       <c r="G26">
-        <v>123.42</v>
+        <v>124.72</v>
       </c>
       <c r="H26">
-        <v>7637</v>
+        <v>7585</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>44025</v>
+        <v>44026</v>
       </c>
       <c r="B27">
-        <v>124.68</v>
+        <v>126.9</v>
       </c>
       <c r="C27">
-        <v>124.72</v>
+        <v>126.92</v>
       </c>
       <c r="D27">
-        <v>125.3</v>
+        <v>124.14</v>
       </c>
       <c r="E27">
-        <v>125.92</v>
+        <v>128.16</v>
       </c>
       <c r="F27">
-        <v>124.04</v>
+        <v>122.94</v>
       </c>
       <c r="G27">
-        <v>124.72</v>
+        <v>126.79657</v>
       </c>
       <c r="H27">
-        <v>7585</v>
+        <v>12439</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>44026</v>
+        <v>44027</v>
       </c>
       <c r="B28">
-        <v>126.9</v>
+        <v>127.5</v>
       </c>
       <c r="C28">
-        <v>126.92</v>
+        <v>127.54</v>
       </c>
       <c r="D28">
-        <v>124.14</v>
+        <v>127.5</v>
       </c>
       <c r="E28">
-        <v>128.16</v>
+        <v>127.86</v>
       </c>
       <c r="F28">
-        <v>122.94</v>
+        <v>124.72</v>
       </c>
       <c r="G28">
-        <v>126.79657</v>
+        <v>126.855</v>
       </c>
       <c r="H28">
-        <v>12439</v>
+        <v>12158</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>44027</v>
+        <v>44028</v>
       </c>
       <c r="B29">
-        <v>127.5</v>
+        <v>127.46</v>
       </c>
       <c r="C29">
         <v>127.54</v>
       </c>
       <c r="D29">
-        <v>127.5</v>
+        <v>127.02</v>
       </c>
       <c r="E29">
-        <v>127.86</v>
+        <v>128.96</v>
       </c>
       <c r="F29">
-        <v>124.72</v>
+        <v>126.84</v>
       </c>
       <c r="G29">
-        <v>126.855</v>
+        <v>127.94</v>
       </c>
       <c r="H29">
-        <v>12158</v>
+        <v>9279</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>44028</v>
+        <v>44029</v>
       </c>
       <c r="B30">
-        <v>127.46</v>
+        <v>129.78</v>
       </c>
       <c r="C30">
-        <v>127.54</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="D30">
-        <v>127.02</v>
+        <v>127.7</v>
       </c>
       <c r="E30">
-        <v>128.96</v>
+        <v>130.47999999999999</v>
       </c>
       <c r="F30">
-        <v>126.84</v>
+        <v>126.2</v>
       </c>
       <c r="G30">
-        <v>127.94</v>
+        <v>129.048</v>
       </c>
       <c r="H30">
-        <v>9279</v>
+        <v>12281</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>44029</v>
+        <v>44032</v>
       </c>
       <c r="B31">
-        <v>129.78</v>
+        <v>129.28</v>
       </c>
       <c r="C31">
-        <v>129.80000000000001</v>
+        <v>129.30000000000001</v>
       </c>
       <c r="D31">
-        <v>127.7</v>
+        <v>129.84</v>
       </c>
       <c r="E31">
-        <v>130.47999999999999</v>
+        <v>130.44</v>
       </c>
       <c r="F31">
-        <v>126.2</v>
+        <v>127.94</v>
       </c>
       <c r="G31">
-        <v>129.048</v>
+        <v>129.28</v>
       </c>
       <c r="H31">
-        <v>12281</v>
+        <v>9003</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="B32">
-        <v>129.28</v>
+        <v>130.32</v>
       </c>
       <c r="C32">
-        <v>129.30000000000001</v>
+        <v>130.34</v>
       </c>
       <c r="D32">
-        <v>129.84</v>
+        <v>129.9</v>
       </c>
       <c r="E32">
-        <v>130.44</v>
+        <v>132.18</v>
       </c>
       <c r="F32">
-        <v>127.94</v>
+        <v>129.22</v>
       </c>
       <c r="G32">
-        <v>129.28</v>
+        <v>129.9</v>
       </c>
       <c r="H32">
-        <v>9003</v>
+        <v>11034</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>